<commit_message>
Schema files are contributed by Infoteria
</commit_message>
<xml_diff>
--- a/doc/vitalsign.xlsx
+++ b/doc/vitalsign.xlsx
@@ -12,14 +12,14 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$H$57</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$H$58</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="101">
   <si>
     <t>Elements</t>
   </si>
@@ -365,22 +365,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>1.3.1</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>1.3.2</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>1.3.3</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>1.3.4</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>?</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -441,10 +425,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>1.3.5</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>?</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -477,6 +457,30 @@
   </si>
   <si>
     <t>dateTime</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>1.4.1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>1.4.2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>1.4.3</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>1.4.4</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>1.4.5</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>1.5</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -898,10 +902,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H57"/>
+  <dimension ref="A1:H58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -956,38 +960,31 @@
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="10" t="s">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A4" s="2"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B5" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="11" t="s">
+      <c r="C5" s="11"/>
+      <c r="D5" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="11" t="s">
         <v>7</v>
-      </c>
-      <c r="F4" s="11"/>
-      <c r="H4" s="4"/>
-    </row>
-    <row r="5" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="10"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>6</v>
       </c>
       <c r="F5" s="11"/>
       <c r="H5" s="4"/>
@@ -996,7 +993,7 @@
       <c r="A6" s="10"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D6" s="11" t="s">
         <v>5</v>
@@ -1004,47 +1001,46 @@
       <c r="E6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="11"/>
+      <c r="H6" s="4"/>
+    </row>
+    <row r="7" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="10"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="11" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="10" t="s">
+    <row r="8" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B8" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" s="11" t="s">
+      <c r="C8" s="11"/>
+      <c r="D8" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="11"/>
-    </row>
-    <row r="8" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="10"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="F8" s="11" t="s">
-        <v>25</v>
-      </c>
+      <c r="F8" s="11"/>
     </row>
     <row r="9" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A9" s="10"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D9" s="11" t="s">
         <v>5</v>
@@ -1052,45 +1048,45 @@
       <c r="E9" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="F9" s="11"/>
+      <c r="F9" s="11" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="10" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="10"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" s="11"/>
+    </row>
+    <row r="11" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B11" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="E10" s="11" t="s">
+      <c r="C11" s="11"/>
+      <c r="D11" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="F10" s="11"/>
-    </row>
-    <row r="11" spans="1:8" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.15">
-      <c r="A11" s="10"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="F11" s="11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="F11" s="11"/>
+    </row>
+    <row r="12" spans="1:8" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.15">
       <c r="A12" s="10"/>
       <c r="B12" s="11"/>
       <c r="C12" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D12" s="11" t="s">
         <v>5</v>
@@ -1098,45 +1094,45 @@
       <c r="E12" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="F12" s="11"/>
+      <c r="F12" s="11" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="13" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="10"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" s="11"/>
+    </row>
+    <row r="14" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B14" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="E13" s="11" t="s">
+      <c r="C14" s="11"/>
+      <c r="D14" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="F13" s="11"/>
-    </row>
-    <row r="14" spans="1:8" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.15">
-      <c r="A14" s="10"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="F14" s="11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="F14" s="11"/>
+    </row>
+    <row r="15" spans="1:8" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.15">
       <c r="A15" s="10"/>
       <c r="B15" s="11"/>
       <c r="C15" s="11" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D15" s="11" t="s">
         <v>5</v>
@@ -1144,374 +1140,390 @@
       <c r="E15" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="F15" s="11"/>
-    </row>
-    <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="H16" s="12"/>
-    </row>
-    <row r="17" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="F15" s="11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="10"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16" s="11"/>
+    </row>
+    <row r="17" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="2" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>69</v>
+        <v>88</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
-      <c r="E17" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="E17" s="1"/>
       <c r="F17" s="1"/>
+      <c r="H17" s="12"/>
     </row>
     <row r="18" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A18" s="2" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C18" s="1"/>
-      <c r="D18" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1" t="s">
-        <v>85</v>
-      </c>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" s="1"/>
     </row>
     <row r="19" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A19" s="2" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E19" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="F19" s="1"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="E19" s="1"/>
+      <c r="F19" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A20" s="2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>7</v>
+        <v>71</v>
       </c>
       <c r="F20" s="1"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A21" s="2" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F21" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="H21" t="s">
-        <v>33</v>
-      </c>
+      <c r="F21" s="1"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A22" s="2" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>12</v>
+        <v>73</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F22" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>82</v>
+      </c>
       <c r="H22" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A23" s="2" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>98</v>
+        <v>12</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E23" s="1"/>
+        <v>5</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="F23" s="1"/>
+      <c r="H23" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A24" s="2">
-        <v>1.3</v>
+      <c r="A24" s="2" t="s">
+        <v>92</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>13</v>
+        <v>93</v>
       </c>
       <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="D24" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E24" s="1"/>
       <c r="F24" s="1"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A25" s="2" t="s">
-        <v>71</v>
+        <v>89</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
       <c r="E25" s="1" t="s">
-        <v>96</v>
+        <v>7</v>
       </c>
       <c r="F25" s="1"/>
-      <c r="H25" s="1" t="s">
-        <v>49</v>
-      </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A26" s="2" t="s">
-        <v>72</v>
+        <v>95</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>58</v>
+        <v>5</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="F26" s="1"/>
       <c r="H26" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A27" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F27" s="1"/>
+      <c r="H27" s="1" t="s">
         <v>48</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="27" x14ac:dyDescent="0.15">
-      <c r="A27" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="27" x14ac:dyDescent="0.15">
       <c r="A28" s="2" t="s">
-        <v>74</v>
+        <v>97</v>
       </c>
       <c r="B28" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="27" x14ac:dyDescent="0.15">
+      <c r="A29" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D28" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="F28" s="1"/>
-      <c r="H28" s="1" t="s">
+      <c r="D29" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F29" s="1"/>
+      <c r="H29" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A29" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="B29" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="C29" s="11"/>
-      <c r="D29" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="E29" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="F29" s="11"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A30" s="10" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="C30" s="11"/>
       <c r="D30" s="11" t="s">
         <v>5</v>
       </c>
       <c r="E30" s="11" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A32" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="F30" s="11"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A31" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="C31" s="11"/>
+      <c r="D31" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E31" s="11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A33" s="6" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A33" s="3" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A34" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A35" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A36" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A37" s="3" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A38" s="3" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A39" s="3" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A40" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A41" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A42" s="3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="42" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A43" s="6" t="s">
+    <row r="43" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A44" s="6" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A44" s="3" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A45" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A46" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A47" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A48" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A49" s="3" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A50" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A51" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A52" s="6" t="s">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A53" s="6" t="s">
         <v>60</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A53" s="3" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A54" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A55" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A56" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A57" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A58" s="3" t="s">
         <v>65</v>
       </c>
     </row>

</xml_diff>